<commit_message>
added report in report directory
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -28,16 +28,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Название ГО</t>
+    <t>Департамент государственных доходов по СКО</t>
   </si>
   <si>
-    <t>ФИО</t>
+    <t>Саржанова Роза Молдашевна</t>
   </si>
   <si>
-    <t>Запрос</t>
+    <t>Консультация по работе в БД Проекты</t>
   </si>
   <si>
-    <t>Емайл</t>
+    <t>sko@sko.kz</t>
   </si>
 </sst>
 </file>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +884,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" display="sko@sko.kz"/>
+    <hyperlink ref="D1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>